<commit_message>
KIBON-963 Sortierung Tagesschulmodule in Statistik
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/TagesschuleOhneFinSit.xlsx
+++ b/ebegu-server/src/main/resources/reporting/TagesschuleOhneFinSit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219C4C09-1A34-425D-8818-C1F5C336BE28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B21AEE-01BD-4770-8BE4-2F0E797755B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -138,7 +138,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -174,17 +174,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -216,7 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -631,7 +620,7 @@
   <dimension ref="A1:DD7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,11 +628,13 @@
     <col min="1" max="2" width="20.7109375"/>
     <col min="3" max="3" width="15.7109375" style="1"/>
     <col min="4" max="5" width="17"/>
-    <col min="6" max="11" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
+    <col min="7" max="11" width="13.28515625" customWidth="1"/>
     <col min="12" max="12" width="13.5703125" customWidth="1"/>
     <col min="13" max="105" width="10.5703125"/>
     <col min="106" max="106" width="10.5703125" customWidth="1"/>
-    <col min="107" max="966" width="10.5703125"/>
+    <col min="107" max="107" width="7.42578125" customWidth="1"/>
+    <col min="108" max="966" width="10.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:108" ht="21" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
KIBON-963 Anpassen Template mit Datum Format und Ändern vom Namen des Excels
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/TagesschuleOhneFinSit.xlsx
+++ b/ebegu-server/src/main/resources/reporting/TagesschuleOhneFinSit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0E5386-3C6A-4C4C-AD04-28BB859EAE91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCF11D2-950C-4C8A-9B73-A2F339225A94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -262,9 +262,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -273,15 +270,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -296,6 +284,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -738,7 +738,7 @@
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:107" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="2"/>
@@ -1162,7 +1162,7 @@
       <c r="DB4" t="s">
         <v>22</v>
       </c>
-      <c r="DC4" s="19"/>
+      <c r="DC4" s="15"/>
     </row>
     <row r="5" spans="1:107" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -1183,125 +1183,125 @@
       <c r="F5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="12" t="s">
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+      <c r="P5" s="17"/>
+      <c r="Q5" s="17"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="17"/>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="17"/>
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="13"/>
-      <c r="AD5" s="13"/>
-      <c r="AE5" s="13"/>
-      <c r="AF5" s="13"/>
-      <c r="AG5" s="13"/>
-      <c r="AH5" s="13"/>
-      <c r="AI5" s="13"/>
-      <c r="AJ5" s="13"/>
-      <c r="AK5" s="13"/>
-      <c r="AL5" s="13"/>
-      <c r="AM5" s="13"/>
-      <c r="AN5" s="13"/>
-      <c r="AO5" s="13"/>
-      <c r="AP5" s="13"/>
-      <c r="AQ5" s="13"/>
-      <c r="AR5" s="13"/>
-      <c r="AS5" s="13"/>
-      <c r="AT5" s="14"/>
-      <c r="AU5" s="12" t="s">
+      <c r="AB5" s="17"/>
+      <c r="AC5" s="17"/>
+      <c r="AD5" s="17"/>
+      <c r="AE5" s="17"/>
+      <c r="AF5" s="17"/>
+      <c r="AG5" s="17"/>
+      <c r="AH5" s="17"/>
+      <c r="AI5" s="17"/>
+      <c r="AJ5" s="17"/>
+      <c r="AK5" s="17"/>
+      <c r="AL5" s="17"/>
+      <c r="AM5" s="17"/>
+      <c r="AN5" s="17"/>
+      <c r="AO5" s="17"/>
+      <c r="AP5" s="17"/>
+      <c r="AQ5" s="17"/>
+      <c r="AR5" s="17"/>
+      <c r="AS5" s="17"/>
+      <c r="AT5" s="18"/>
+      <c r="AU5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="AV5" s="13"/>
-      <c r="AW5" s="13"/>
-      <c r="AX5" s="13"/>
-      <c r="AY5" s="13"/>
-      <c r="AZ5" s="13"/>
-      <c r="BA5" s="13"/>
-      <c r="BB5" s="13"/>
-      <c r="BC5" s="13"/>
-      <c r="BD5" s="13"/>
-      <c r="BE5" s="13"/>
-      <c r="BF5" s="13"/>
-      <c r="BG5" s="13"/>
-      <c r="BH5" s="13"/>
-      <c r="BI5" s="13"/>
-      <c r="BJ5" s="13"/>
-      <c r="BK5" s="13"/>
-      <c r="BL5" s="13"/>
-      <c r="BM5" s="13"/>
-      <c r="BN5" s="14"/>
-      <c r="BO5" s="12" t="s">
+      <c r="AV5" s="17"/>
+      <c r="AW5" s="17"/>
+      <c r="AX5" s="17"/>
+      <c r="AY5" s="17"/>
+      <c r="AZ5" s="17"/>
+      <c r="BA5" s="17"/>
+      <c r="BB5" s="17"/>
+      <c r="BC5" s="17"/>
+      <c r="BD5" s="17"/>
+      <c r="BE5" s="17"/>
+      <c r="BF5" s="17"/>
+      <c r="BG5" s="17"/>
+      <c r="BH5" s="17"/>
+      <c r="BI5" s="17"/>
+      <c r="BJ5" s="17"/>
+      <c r="BK5" s="17"/>
+      <c r="BL5" s="17"/>
+      <c r="BM5" s="17"/>
+      <c r="BN5" s="18"/>
+      <c r="BO5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="BP5" s="13"/>
-      <c r="BQ5" s="13"/>
-      <c r="BR5" s="13"/>
-      <c r="BS5" s="13"/>
-      <c r="BT5" s="13"/>
-      <c r="BU5" s="13"/>
-      <c r="BV5" s="13"/>
-      <c r="BW5" s="13"/>
-      <c r="BX5" s="13"/>
-      <c r="BY5" s="13"/>
-      <c r="BZ5" s="13"/>
-      <c r="CA5" s="13"/>
-      <c r="CB5" s="13"/>
-      <c r="CC5" s="13"/>
-      <c r="CD5" s="13"/>
-      <c r="CE5" s="13"/>
-      <c r="CF5" s="13"/>
-      <c r="CG5" s="13"/>
-      <c r="CH5" s="14"/>
-      <c r="CI5" s="12" t="s">
+      <c r="BP5" s="17"/>
+      <c r="BQ5" s="17"/>
+      <c r="BR5" s="17"/>
+      <c r="BS5" s="17"/>
+      <c r="BT5" s="17"/>
+      <c r="BU5" s="17"/>
+      <c r="BV5" s="17"/>
+      <c r="BW5" s="17"/>
+      <c r="BX5" s="17"/>
+      <c r="BY5" s="17"/>
+      <c r="BZ5" s="17"/>
+      <c r="CA5" s="17"/>
+      <c r="CB5" s="17"/>
+      <c r="CC5" s="17"/>
+      <c r="CD5" s="17"/>
+      <c r="CE5" s="17"/>
+      <c r="CF5" s="17"/>
+      <c r="CG5" s="17"/>
+      <c r="CH5" s="18"/>
+      <c r="CI5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="CJ5" s="13"/>
-      <c r="CK5" s="13"/>
-      <c r="CL5" s="13"/>
-      <c r="CM5" s="13"/>
-      <c r="CN5" s="13"/>
-      <c r="CO5" s="13"/>
-      <c r="CP5" s="13"/>
-      <c r="CQ5" s="13"/>
-      <c r="CR5" s="13"/>
-      <c r="CS5" s="13"/>
-      <c r="CT5" s="13"/>
-      <c r="CU5" s="13"/>
-      <c r="CV5" s="13"/>
-      <c r="CW5" s="13"/>
-      <c r="CX5" s="13"/>
-      <c r="CY5" s="13"/>
-      <c r="CZ5" s="13"/>
-      <c r="DA5" s="13"/>
-      <c r="DB5" s="13"/>
-      <c r="DC5" s="17"/>
+      <c r="CJ5" s="17"/>
+      <c r="CK5" s="17"/>
+      <c r="CL5" s="17"/>
+      <c r="CM5" s="17"/>
+      <c r="CN5" s="17"/>
+      <c r="CO5" s="17"/>
+      <c r="CP5" s="17"/>
+      <c r="CQ5" s="17"/>
+      <c r="CR5" s="17"/>
+      <c r="CS5" s="17"/>
+      <c r="CT5" s="17"/>
+      <c r="CU5" s="17"/>
+      <c r="CV5" s="17"/>
+      <c r="CW5" s="17"/>
+      <c r="CX5" s="17"/>
+      <c r="CY5" s="17"/>
+      <c r="CZ5" s="17"/>
+      <c r="DA5" s="17"/>
+      <c r="DB5" s="17"/>
+      <c r="DC5" s="13"/>
     </row>
     <row r="6" spans="1:107" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
       <c r="G6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1599,331 +1599,331 @@
       <c r="DA6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="DB6" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="DC6" s="17"/>
+      <c r="DB6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="DC6" s="13"/>
     </row>
     <row r="7" spans="1:107" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="O7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="P7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="R7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="S7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="T7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="U7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="V7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="W7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="X7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AF7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AG7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AH7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AI7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AJ7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AK7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AL7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AM7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AN7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AO7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AP7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AQ7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AR7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AS7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AT7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AU7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AV7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AW7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AX7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AY7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AZ7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BA7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BB7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BC7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BD7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BE7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BF7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BG7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BH7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BI7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BJ7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BK7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BL7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BM7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BN7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BO7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BP7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BQ7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BR7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BS7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BT7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BU7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BV7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BW7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BX7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BY7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="BZ7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CA7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CB7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CC7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CD7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CE7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CF7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CG7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CH7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CI7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CJ7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CK7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CL7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CM7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CN7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CO7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CP7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CQ7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CR7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CS7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CT7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CU7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CV7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CW7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CX7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CY7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="CZ7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="DA7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="DB7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="DC7" s="18" t="s">
+      <c r="G7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="T7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="U7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="V7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="W7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="X7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AH7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AM7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AN7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AQ7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AU7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AV7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AW7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AY7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="AZ7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BA7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BC7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BD7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BE7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BF7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BG7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BH7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BI7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BJ7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BK7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BL7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BM7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BN7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BO7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BP7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BQ7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BR7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BS7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BT7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BU7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BV7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BW7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BX7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BY7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="BZ7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CA7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CB7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CC7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CD7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CE7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CF7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CG7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CH7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CI7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CJ7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CK7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CL7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CM7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CN7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CO7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CP7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CQ7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CR7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CS7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CT7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CU7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CV7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CW7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CX7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CY7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="CZ7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="DA7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="DB7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="DC7" s="14" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
KIBON-1218 Summen zu Tagesschule Statistik hinzugefügt. Nicht freigegebene Gesuche nicht mehr sichtbar
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/TagesschuleOhneFinSit.xlsx
+++ b/ebegu-server/src/main/resources/reporting/TagesschuleOhneFinSit.xlsx
@@ -1,20 +1,123 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCF11D2-950C-4C8A-9B73-A2F339225A94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0523F2E8-CAE6-46C6-9D3F-2EA67B212B1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="angemeldet1">Data!$H$7</definedName>
+    <definedName name="angemeldet10">Data!$Q$7</definedName>
+    <definedName name="angemeldet100">Data!$DC$7</definedName>
+    <definedName name="angemeldet11">Data!$R$7</definedName>
+    <definedName name="angemeldet12">Data!$S$7</definedName>
+    <definedName name="angemeldet13">Data!$T$7</definedName>
+    <definedName name="angemeldet14">Data!$U$7</definedName>
+    <definedName name="angemeldet15">Data!$V$7</definedName>
+    <definedName name="angemeldet16">Data!$W$7</definedName>
+    <definedName name="angemeldet17">Data!$X$7</definedName>
+    <definedName name="angemeldet18">Data!$Y$7</definedName>
+    <definedName name="angemeldet19">Data!$Z$7</definedName>
+    <definedName name="angemeldet2">Data!$I$7</definedName>
+    <definedName name="angemeldet20">Data!$AA$7</definedName>
+    <definedName name="angemeldet21">Data!$AB$7</definedName>
+    <definedName name="angemeldet22">Data!$AC$7</definedName>
+    <definedName name="angemeldet23">Data!$AD$7</definedName>
+    <definedName name="angemeldet24">Data!$AE$7</definedName>
+    <definedName name="angemeldet25">Data!$AF$7</definedName>
+    <definedName name="angemeldet26">Data!$AG$7</definedName>
+    <definedName name="angemeldet27">Data!$AH$7</definedName>
+    <definedName name="angemeldet28">Data!$AI$7</definedName>
+    <definedName name="angemeldet29">Data!$AJ$7</definedName>
+    <definedName name="angemeldet3">Data!$J$7</definedName>
+    <definedName name="angemeldet30">Data!$AK$7</definedName>
+    <definedName name="angemeldet31">Data!$AL$7</definedName>
+    <definedName name="angemeldet32">Data!$AM$7</definedName>
+    <definedName name="angemeldet33">Data!$AN$7</definedName>
+    <definedName name="angemeldet34">Data!$AO$7</definedName>
+    <definedName name="angemeldet35">Data!$AP$7</definedName>
+    <definedName name="angemeldet36">Data!$AQ$7</definedName>
+    <definedName name="angemeldet37">Data!$AR$7</definedName>
+    <definedName name="angemeldet38">Data!$AS$7</definedName>
+    <definedName name="angemeldet39">Data!$AT$7</definedName>
+    <definedName name="angemeldet4">Data!$K$7</definedName>
+    <definedName name="angemeldet40">Data!$AU$7</definedName>
+    <definedName name="angemeldet41">Data!$AV$7</definedName>
+    <definedName name="angemeldet42">Data!$AW$7</definedName>
+    <definedName name="angemeldet43">Data!$AX$7</definedName>
+    <definedName name="angemeldet44">Data!$AY$7</definedName>
+    <definedName name="angemeldet45">Data!$AZ$7</definedName>
+    <definedName name="angemeldet46">Data!$BA$7</definedName>
+    <definedName name="angemeldet47">Data!$BB$7</definedName>
+    <definedName name="angemeldet48">Data!$BC$7</definedName>
+    <definedName name="angemeldet49">Data!$BD$7</definedName>
+    <definedName name="angemeldet5">Data!$L$7</definedName>
+    <definedName name="angemeldet50">Data!$BE$7</definedName>
+    <definedName name="angemeldet51">Data!$BF$7</definedName>
+    <definedName name="angemeldet52">Data!$BG$7</definedName>
+    <definedName name="angemeldet53">Data!$BH$7</definedName>
+    <definedName name="angemeldet54">Data!$BI$7</definedName>
+    <definedName name="angemeldet55">Data!$BJ$7</definedName>
+    <definedName name="angemeldet56">Data!$BK$7</definedName>
+    <definedName name="angemeldet57">Data!$BL$7</definedName>
+    <definedName name="angemeldet58">Data!$BM$7</definedName>
+    <definedName name="angemeldet59">Data!$BN$7</definedName>
+    <definedName name="angemeldet6">Data!$M$7</definedName>
+    <definedName name="angemeldet60">Data!$BO$7</definedName>
+    <definedName name="angemeldet61">Data!$BP$7</definedName>
+    <definedName name="angemeldet62">Data!$BQ$7</definedName>
+    <definedName name="angemeldet63">Data!$BR$7</definedName>
+    <definedName name="angemeldet64">Data!$BS$7</definedName>
+    <definedName name="angemeldet65">Data!$BT$7</definedName>
+    <definedName name="angemeldet66">Data!$BU$7</definedName>
+    <definedName name="angemeldet67">Data!$BV$7</definedName>
+    <definedName name="angemeldet68">Data!$BW$7</definedName>
+    <definedName name="angemeldet69">Data!$BX$7</definedName>
+    <definedName name="angemeldet7">Data!$N$7</definedName>
+    <definedName name="angemeldet70">Data!$BY$7</definedName>
+    <definedName name="angemeldet71">Data!$BZ$7</definedName>
+    <definedName name="angemeldet72">Data!$CA$7</definedName>
+    <definedName name="angemeldet73">Data!$CB$7</definedName>
+    <definedName name="angemeldet74">Data!$CC$7</definedName>
+    <definedName name="angemeldet75">Data!$CD$7</definedName>
+    <definedName name="angemeldet76">Data!$CE$7</definedName>
+    <definedName name="angemeldet77">Data!$CF$7</definedName>
+    <definedName name="angemeldet78">Data!$CG$7</definedName>
+    <definedName name="angemeldet79">Data!$CH$7</definedName>
+    <definedName name="angemeldet8">Data!$O$7</definedName>
+    <definedName name="angemeldet80">Data!$CI$7</definedName>
+    <definedName name="angemeldet81">Data!$CJ$7</definedName>
+    <definedName name="angemeldet82">Data!$CK$7</definedName>
+    <definedName name="angemeldet83">Data!$CL$7</definedName>
+    <definedName name="angemeldet84">Data!$CM$7</definedName>
+    <definedName name="angemeldet85">Data!$CN$7</definedName>
+    <definedName name="angemeldet86">Data!$CO$7</definedName>
+    <definedName name="angemeldet87">Data!$CP$7</definedName>
+    <definedName name="angemeldet88">Data!$CQ$7</definedName>
+    <definedName name="angemeldet89">Data!$CR$7</definedName>
+    <definedName name="angemeldet9">Data!$P$7</definedName>
+    <definedName name="angemeldet90">Data!$CS$7</definedName>
+    <definedName name="angemeldet91">Data!$CT$7</definedName>
+    <definedName name="angemeldet92">Data!$CU$7</definedName>
+    <definedName name="angemeldet93">Data!$CV$7</definedName>
+    <definedName name="angemeldet94">Data!$CW$7</definedName>
+    <definedName name="angemeldet95">Data!$CX$7</definedName>
+    <definedName name="angemeldet96">Data!$CY$7</definedName>
+    <definedName name="angemeldet97">Data!$CZ$7</definedName>
+    <definedName name="angemeldet98">Data!$DA$7</definedName>
+    <definedName name="angemeldet99">Data!$DB$7</definedName>
+    <definedName name="statusKategorie">Data!$G$7</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="46">
   <si>
     <t>{statusTitle}</t>
   </si>
@@ -102,6 +205,75 @@
   </si>
   <si>
     <t>{repeatCol5}</t>
+  </si>
+  <si>
+    <t>Anzahl bestätigte Anmeldungen</t>
+  </si>
+  <si>
+    <t>Anzahl abgelehnte Anmeldungen</t>
+  </si>
+  <si>
+    <t>Anzahl offene Anmeldungen</t>
+  </si>
+  <si>
+    <t>In Bearbeitung</t>
+  </si>
+  <si>
+    <t>Anmeldung ausgelöst</t>
+  </si>
+  <si>
+    <t>Anmeldung übernommen</t>
+  </si>
+  <si>
+    <t>Anmeldung abgelehnt</t>
+  </si>
+  <si>
+    <t>Falsche Institution</t>
+  </si>
+  <si>
+    <t>Module akzeptiert</t>
+  </si>
+  <si>
+    <t>En traitement</t>
+  </si>
+  <si>
+    <t>Inscription en cours</t>
+  </si>
+  <si>
+    <t>Inscription reprise</t>
+  </si>
+  <si>
+    <t>Inscription refusée</t>
+  </si>
+  <si>
+    <t>Institution erronée</t>
+  </si>
+  <si>
+    <t>Modules acceptés</t>
+  </si>
+  <si>
+    <t>Status offen</t>
+  </si>
+  <si>
+    <t>OFFEN</t>
+  </si>
+  <si>
+    <t>Status abgelehnt</t>
+  </si>
+  <si>
+    <t>ABGELEHNT</t>
+  </si>
+  <si>
+    <t>Status bestätigt</t>
+  </si>
+  <si>
+    <t>BESTÄTIGT</t>
+  </si>
+  <si>
+    <t>Anzahl nicht freigegebene Anmeldungen</t>
+  </si>
+  <si>
+    <t>{nichtFreigegebenAnzahl}</t>
   </si>
 </sst>
 </file>
@@ -136,7 +308,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,6 +319,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -233,21 +411,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -274,9 +450,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -287,15 +460,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -702,12 +885,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Tabelle1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DC7"/>
+  <dimension ref="A1:DD28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -715,14 +900,15 @@
     <col min="3" max="3" width="15.7109375" style="1"/>
     <col min="4" max="5" width="17"/>
     <col min="6" max="6" width="33.140625" customWidth="1"/>
-    <col min="7" max="11" width="13.28515625" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
-    <col min="13" max="105" width="10.5703125"/>
-    <col min="106" max="106" width="8.85546875" customWidth="1"/>
-    <col min="107" max="965" width="10.5703125"/>
+    <col min="7" max="7" width="33.140625" hidden="1" customWidth="1"/>
+    <col min="8" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="14" max="106" width="10.5703125"/>
+    <col min="107" max="107" width="8.85546875" customWidth="1"/>
+    <col min="108" max="966" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:107" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:108" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -736,8 +922,9 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:107" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:108" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>15</v>
       </c>
@@ -751,8 +938,9 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:107" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:108" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
@@ -859,12 +1047,10 @@
       <c r="CZ3" s="2"/>
       <c r="DA3" s="2"/>
       <c r="DB3" s="2"/>
+      <c r="DC3" s="2"/>
     </row>
-    <row r="4" spans="1:107" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:108" x14ac:dyDescent="0.25">
       <c r="C4"/>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
       <c r="H4" t="s">
         <v>18</v>
       </c>
@@ -923,7 +1109,7 @@
         <v>18</v>
       </c>
       <c r="AA4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AB4" t="s">
         <v>19</v>
@@ -983,7 +1169,7 @@
         <v>19</v>
       </c>
       <c r="AU4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AV4" t="s">
         <v>20</v>
@@ -1043,7 +1229,7 @@
         <v>20</v>
       </c>
       <c r="BO4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="BP4" t="s">
         <v>21</v>
@@ -1103,7 +1289,7 @@
         <v>21</v>
       </c>
       <c r="CI4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="CJ4" t="s">
         <v>22</v>
@@ -1162,9 +1348,12 @@
       <c r="DB4" t="s">
         <v>22</v>
       </c>
-      <c r="DC4" s="15"/>
+      <c r="DC4" t="s">
+        <v>22</v>
+      </c>
+      <c r="DD4" s="14"/>
     </row>
-    <row r="5" spans="1:107" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:108" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -1183,128 +1372,127 @@
       <c r="F5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="15"/>
+      <c r="H5" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="17"/>
-      <c r="V5" s="17"/>
-      <c r="W5" s="17"/>
-      <c r="X5" s="17"/>
-      <c r="Y5" s="17"/>
-      <c r="Z5" s="18"/>
-      <c r="AA5" s="16" t="s">
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="21"/>
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="21"/>
+      <c r="AA5" s="22"/>
+      <c r="AB5" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="AB5" s="17"/>
-      <c r="AC5" s="17"/>
-      <c r="AD5" s="17"/>
-      <c r="AE5" s="17"/>
-      <c r="AF5" s="17"/>
-      <c r="AG5" s="17"/>
-      <c r="AH5" s="17"/>
-      <c r="AI5" s="17"/>
-      <c r="AJ5" s="17"/>
-      <c r="AK5" s="17"/>
-      <c r="AL5" s="17"/>
-      <c r="AM5" s="17"/>
-      <c r="AN5" s="17"/>
-      <c r="AO5" s="17"/>
-      <c r="AP5" s="17"/>
-      <c r="AQ5" s="17"/>
-      <c r="AR5" s="17"/>
-      <c r="AS5" s="17"/>
-      <c r="AT5" s="18"/>
-      <c r="AU5" s="16" t="s">
+      <c r="AC5" s="21"/>
+      <c r="AD5" s="21"/>
+      <c r="AE5" s="21"/>
+      <c r="AF5" s="21"/>
+      <c r="AG5" s="21"/>
+      <c r="AH5" s="21"/>
+      <c r="AI5" s="21"/>
+      <c r="AJ5" s="21"/>
+      <c r="AK5" s="21"/>
+      <c r="AL5" s="21"/>
+      <c r="AM5" s="21"/>
+      <c r="AN5" s="21"/>
+      <c r="AO5" s="21"/>
+      <c r="AP5" s="21"/>
+      <c r="AQ5" s="21"/>
+      <c r="AR5" s="21"/>
+      <c r="AS5" s="21"/>
+      <c r="AT5" s="21"/>
+      <c r="AU5" s="22"/>
+      <c r="AV5" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="AV5" s="17"/>
-      <c r="AW5" s="17"/>
-      <c r="AX5" s="17"/>
-      <c r="AY5" s="17"/>
-      <c r="AZ5" s="17"/>
-      <c r="BA5" s="17"/>
-      <c r="BB5" s="17"/>
-      <c r="BC5" s="17"/>
-      <c r="BD5" s="17"/>
-      <c r="BE5" s="17"/>
-      <c r="BF5" s="17"/>
-      <c r="BG5" s="17"/>
-      <c r="BH5" s="17"/>
-      <c r="BI5" s="17"/>
-      <c r="BJ5" s="17"/>
-      <c r="BK5" s="17"/>
-      <c r="BL5" s="17"/>
-      <c r="BM5" s="17"/>
-      <c r="BN5" s="18"/>
-      <c r="BO5" s="16" t="s">
+      <c r="AW5" s="21"/>
+      <c r="AX5" s="21"/>
+      <c r="AY5" s="21"/>
+      <c r="AZ5" s="21"/>
+      <c r="BA5" s="21"/>
+      <c r="BB5" s="21"/>
+      <c r="BC5" s="21"/>
+      <c r="BD5" s="21"/>
+      <c r="BE5" s="21"/>
+      <c r="BF5" s="21"/>
+      <c r="BG5" s="21"/>
+      <c r="BH5" s="21"/>
+      <c r="BI5" s="21"/>
+      <c r="BJ5" s="21"/>
+      <c r="BK5" s="21"/>
+      <c r="BL5" s="21"/>
+      <c r="BM5" s="21"/>
+      <c r="BN5" s="21"/>
+      <c r="BO5" s="22"/>
+      <c r="BP5" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="BP5" s="17"/>
-      <c r="BQ5" s="17"/>
-      <c r="BR5" s="17"/>
-      <c r="BS5" s="17"/>
-      <c r="BT5" s="17"/>
-      <c r="BU5" s="17"/>
-      <c r="BV5" s="17"/>
-      <c r="BW5" s="17"/>
-      <c r="BX5" s="17"/>
-      <c r="BY5" s="17"/>
-      <c r="BZ5" s="17"/>
-      <c r="CA5" s="17"/>
-      <c r="CB5" s="17"/>
-      <c r="CC5" s="17"/>
-      <c r="CD5" s="17"/>
-      <c r="CE5" s="17"/>
-      <c r="CF5" s="17"/>
-      <c r="CG5" s="17"/>
-      <c r="CH5" s="18"/>
-      <c r="CI5" s="16" t="s">
+      <c r="BQ5" s="21"/>
+      <c r="BR5" s="21"/>
+      <c r="BS5" s="21"/>
+      <c r="BT5" s="21"/>
+      <c r="BU5" s="21"/>
+      <c r="BV5" s="21"/>
+      <c r="BW5" s="21"/>
+      <c r="BX5" s="21"/>
+      <c r="BY5" s="21"/>
+      <c r="BZ5" s="21"/>
+      <c r="CA5" s="21"/>
+      <c r="CB5" s="21"/>
+      <c r="CC5" s="21"/>
+      <c r="CD5" s="21"/>
+      <c r="CE5" s="21"/>
+      <c r="CF5" s="21"/>
+      <c r="CG5" s="21"/>
+      <c r="CH5" s="21"/>
+      <c r="CI5" s="22"/>
+      <c r="CJ5" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="CJ5" s="17"/>
-      <c r="CK5" s="17"/>
-      <c r="CL5" s="17"/>
-      <c r="CM5" s="17"/>
-      <c r="CN5" s="17"/>
-      <c r="CO5" s="17"/>
-      <c r="CP5" s="17"/>
-      <c r="CQ5" s="17"/>
-      <c r="CR5" s="17"/>
-      <c r="CS5" s="17"/>
-      <c r="CT5" s="17"/>
-      <c r="CU5" s="17"/>
-      <c r="CV5" s="17"/>
-      <c r="CW5" s="17"/>
-      <c r="CX5" s="17"/>
-      <c r="CY5" s="17"/>
-      <c r="CZ5" s="17"/>
-      <c r="DA5" s="17"/>
-      <c r="DB5" s="17"/>
-      <c r="DC5" s="13"/>
+      <c r="CK5" s="21"/>
+      <c r="CL5" s="21"/>
+      <c r="CM5" s="21"/>
+      <c r="CN5" s="21"/>
+      <c r="CO5" s="21"/>
+      <c r="CP5" s="21"/>
+      <c r="CQ5" s="21"/>
+      <c r="CR5" s="21"/>
+      <c r="CS5" s="21"/>
+      <c r="CT5" s="21"/>
+      <c r="CU5" s="21"/>
+      <c r="CV5" s="21"/>
+      <c r="CW5" s="21"/>
+      <c r="CX5" s="21"/>
+      <c r="CY5" s="21"/>
+      <c r="CZ5" s="21"/>
+      <c r="DA5" s="21"/>
+      <c r="DB5" s="21"/>
+      <c r="DC5" s="21"/>
+      <c r="DD5" s="12"/>
     </row>
-    <row r="6" spans="1:107" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:108" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="G6" s="8"/>
       <c r="H6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1599,19 +1787,22 @@
       <c r="DA6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="DB6" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="DC6" s="13"/>
+      <c r="DB6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="DC6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="DD6" s="12"/>
     </row>
-    <row r="7" spans="1:107" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="16" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -1623,8 +1814,9 @@
       <c r="F7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>13</v>
+      <c r="G7" s="6" t="e">
+        <f>VLOOKUP(F7,$A$13:$B$24,2,FALSE)</f>
+        <v>#N/A</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>13</v>
@@ -1920,20 +2112,1514 @@
       <c r="DA7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="DB7" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="DC7" s="14" t="s">
+      <c r="DB7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="DC7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="DD7" s="13" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="17">
+        <f>COUNTIF(statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17">
+        <f>COUNTIFS(angemeldet1,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="17">
+        <f>COUNTIFS(angemeldet2,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="17">
+        <f>COUNTIFS(angemeldet3,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="K8" s="17">
+        <f>COUNTIFS(angemeldet4,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="17">
+        <f>COUNTIFS(angemeldet5,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="17">
+        <f>COUNTIFS(angemeldet6,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="17">
+        <f>COUNTIFS(angemeldet7,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="17">
+        <f>COUNTIFS(angemeldet8,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="17">
+        <f>COUNTIFS(angemeldet9,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="17">
+        <f>COUNTIFS(angemeldet10,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="17">
+        <f>COUNTIFS(angemeldet11,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="S8" s="17">
+        <f>COUNTIFS(angemeldet12,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="T8" s="17">
+        <f>COUNTIFS(angemeldet13,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="U8" s="17">
+        <f>COUNTIFS(angemeldet14,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="V8" s="17">
+        <f>COUNTIFS(angemeldet15,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="W8" s="17">
+        <f>COUNTIFS(angemeldet16,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="X8" s="17">
+        <f>COUNTIFS(angemeldet17,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="Y8" s="17">
+        <f>COUNTIFS(angemeldet18,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="Z8" s="17">
+        <f>COUNTIFS(angemeldet19,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="17">
+        <f>COUNTIFS(angemeldet20,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AB8" s="17">
+        <f>COUNTIFS(angemeldet21,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AC8" s="17">
+        <f>COUNTIFS(angemeldet22,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AD8" s="17">
+        <f>COUNTIFS(angemeldet23,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AE8" s="17">
+        <f>COUNTIFS(angemeldet24,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AF8" s="17">
+        <f>COUNTIFS(angemeldet25,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AG8" s="17">
+        <f>COUNTIFS(angemeldet26,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AH8" s="17">
+        <f>COUNTIFS(angemeldet27,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AI8" s="17">
+        <f>COUNTIFS(angemeldet28,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="17">
+        <f>COUNTIFS(angemeldet29,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AK8" s="17">
+        <f>COUNTIFS(angemeldet30,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AL8" s="17">
+        <f>COUNTIFS(angemeldet31,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AM8" s="17">
+        <f>COUNTIFS(angemeldet32,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AN8" s="17">
+        <f>COUNTIFS(angemeldet33,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AO8" s="17">
+        <f>COUNTIFS(angemeldet34,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AP8" s="17">
+        <f>COUNTIFS(angemeldet35,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="17">
+        <f>COUNTIFS(angemeldet36,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AR8" s="17">
+        <f>COUNTIFS(angemeldet37,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AS8" s="17">
+        <f>COUNTIFS(angemeldet38,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AT8" s="17">
+        <f>COUNTIFS(angemeldet39,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AU8" s="17">
+        <f>COUNTIFS(angemeldet40,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AV8" s="17">
+        <f>COUNTIFS(angemeldet41,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AW8" s="17">
+        <f>COUNTIFS(angemeldet42,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AX8" s="17">
+        <f>COUNTIFS(angemeldet43,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AY8" s="17">
+        <f>COUNTIFS(angemeldet44,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="AZ8" s="17">
+        <f>COUNTIFS(angemeldet45,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BA8" s="17">
+        <f>COUNTIFS(angemeldet46,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BB8" s="17">
+        <f>COUNTIFS(angemeldet47,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BC8" s="17">
+        <f>COUNTIFS(angemeldet48,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BD8" s="17">
+        <f>COUNTIFS(angemeldet49,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BE8" s="17">
+        <f>COUNTIFS(angemeldet50,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BF8" s="17">
+        <f>COUNTIFS(angemeldet51,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BG8" s="17">
+        <f>COUNTIFS(angemeldet52,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BH8" s="17">
+        <f>COUNTIFS(angemeldet53,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BI8" s="17">
+        <f>COUNTIFS(angemeldet54,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BJ8" s="17">
+        <f>COUNTIFS(angemeldet55,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BK8" s="17">
+        <f>COUNTIFS(angemeldet56,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BL8" s="17">
+        <f>COUNTIFS(angemeldet57,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BM8" s="17">
+        <f>COUNTIFS(angemeldet58,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BN8" s="17">
+        <f>COUNTIFS(angemeldet59,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BO8" s="17">
+        <f>COUNTIFS(angemeldet60,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BP8" s="17">
+        <f>COUNTIFS(angemeldet61,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BQ8" s="17">
+        <f>COUNTIFS(angemeldet62,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BR8" s="17">
+        <f>COUNTIFS(angemeldet63,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BS8" s="17">
+        <f>COUNTIFS(angemeldet64,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BT8" s="17">
+        <f>COUNTIFS(angemeldet65,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BU8" s="17">
+        <f>COUNTIFS(angemeldet66,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BV8" s="17">
+        <f>COUNTIFS(angemeldet67,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BW8" s="17">
+        <f>COUNTIFS(angemeldet68,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BX8" s="17">
+        <f>COUNTIFS(angemeldet69,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BY8" s="17">
+        <f>COUNTIFS(angemeldet70,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="BZ8" s="17">
+        <f>COUNTIFS(angemeldet71,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CA8" s="17">
+        <f>COUNTIFS(angemeldet72,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CB8" s="17">
+        <f>COUNTIFS(angemeldet73,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CC8" s="17">
+        <f>COUNTIFS(angemeldet74,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CD8" s="17">
+        <f>COUNTIFS(angemeldet75,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CE8" s="17">
+        <f>COUNTIFS(angemeldet76,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CF8" s="17">
+        <f>COUNTIFS(angemeldet77,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CG8" s="17">
+        <f>COUNTIFS(angemeldet78,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CH8" s="17">
+        <f>COUNTIFS(angemeldet79,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CI8" s="17">
+        <f>COUNTIFS(angemeldet80,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CJ8" s="17">
+        <f>COUNTIFS(angemeldet81,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CK8" s="17">
+        <f>COUNTIFS(angemeldet82,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CL8" s="17">
+        <f>COUNTIFS(angemeldet83,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CM8" s="17">
+        <f>COUNTIFS(angemeldet84,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CN8" s="17">
+        <f>COUNTIFS(angemeldet85,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CO8" s="17">
+        <f>COUNTIFS(angemeldet86,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CP8" s="17">
+        <f>COUNTIFS(angemeldet87,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CQ8" s="17">
+        <f>COUNTIFS(angemeldet88,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CR8" s="17">
+        <f>COUNTIFS(angemeldet89,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CS8" s="17">
+        <f>COUNTIFS(angemeldet90,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CT8" s="17">
+        <f>COUNTIFS(angemeldet91,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CU8" s="17">
+        <f>COUNTIFS(angemeldet92,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CV8" s="17">
+        <f>COUNTIFS(angemeldet93,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CW8" s="17">
+        <f>COUNTIFS(angemeldet94,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CX8" s="17">
+        <f>COUNTIFS(angemeldet95,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CY8" s="17">
+        <f>COUNTIFS(angemeldet96,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="CZ8" s="17">
+        <f>COUNTIFS(angemeldet97,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="DA8" s="17">
+        <f>COUNTIFS(angemeldet98,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="DB8" s="17">
+        <f>COUNTIFS(angemeldet99,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+      <c r="DC8" s="17">
+        <f>COUNTIFS(angemeldet100,"X",statusKategorie,$B$28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="17">
+        <f>COUNTIF(statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17">
+        <f>COUNTIFS(angemeldet1,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="17">
+        <f>COUNTIFS(angemeldet2,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="17">
+        <f>COUNTIFS(angemeldet3,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="17">
+        <f>COUNTIFS(angemeldet4,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="17">
+        <f>COUNTIFS(angemeldet5,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="17">
+        <f>COUNTIFS(angemeldet6,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="17">
+        <f>COUNTIFS(angemeldet7,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="17">
+        <f>COUNTIFS(angemeldet8,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="17">
+        <f>COUNTIFS(angemeldet9,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="17">
+        <f>COUNTIFS(angemeldet10,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="R9" s="17">
+        <f>COUNTIFS(angemeldet11,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="S9" s="17">
+        <f>COUNTIFS(angemeldet12,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="T9" s="17">
+        <f>COUNTIFS(angemeldet13,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="U9" s="17">
+        <f>COUNTIFS(angemeldet14,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="V9" s="17">
+        <f>COUNTIFS(angemeldet15,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="W9" s="17">
+        <f>COUNTIFS(angemeldet16,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="X9" s="17">
+        <f>COUNTIFS(angemeldet17,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="Y9" s="17">
+        <f>COUNTIFS(angemeldet18,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="Z9" s="17">
+        <f>COUNTIFS(angemeldet19,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AA9" s="17">
+        <f>COUNTIFS(angemeldet20,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AB9" s="17">
+        <f>COUNTIFS(angemeldet21,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AC9" s="17">
+        <f>COUNTIFS(angemeldet22,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AD9" s="17">
+        <f>COUNTIFS(angemeldet23,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AE9" s="17">
+        <f>COUNTIFS(angemeldet24,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AF9" s="17">
+        <f>COUNTIFS(angemeldet25,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AG9" s="17">
+        <f>COUNTIFS(angemeldet26,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AH9" s="17">
+        <f>COUNTIFS(angemeldet27,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AI9" s="17">
+        <f>COUNTIFS(angemeldet28,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="17">
+        <f>COUNTIFS(angemeldet29,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AK9" s="17">
+        <f>COUNTIFS(angemeldet30,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AL9" s="17">
+        <f>COUNTIFS(angemeldet31,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AM9" s="17">
+        <f>COUNTIFS(angemeldet32,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AN9" s="17">
+        <f>COUNTIFS(angemeldet33,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AO9" s="17">
+        <f>COUNTIFS(angemeldet34,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AP9" s="17">
+        <f>COUNTIFS(angemeldet35,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="17">
+        <f>COUNTIFS(angemeldet36,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AR9" s="17">
+        <f>COUNTIFS(angemeldet37,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AS9" s="17">
+        <f>COUNTIFS(angemeldet38,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AT9" s="17">
+        <f>COUNTIFS(angemeldet39,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AU9" s="17">
+        <f>COUNTIFS(angemeldet40,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AV9" s="17">
+        <f>COUNTIFS(angemeldet41,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AW9" s="17">
+        <f>COUNTIFS(angemeldet42,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AX9" s="17">
+        <f>COUNTIFS(angemeldet43,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AY9" s="17">
+        <f>COUNTIFS(angemeldet44,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="AZ9" s="17">
+        <f>COUNTIFS(angemeldet45,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BA9" s="17">
+        <f>COUNTIFS(angemeldet46,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BB9" s="17">
+        <f>COUNTIFS(angemeldet47,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BC9" s="17">
+        <f>COUNTIFS(angemeldet48,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BD9" s="17">
+        <f>COUNTIFS(angemeldet49,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BE9" s="17">
+        <f>COUNTIFS(angemeldet50,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BF9" s="17">
+        <f>COUNTIFS(angemeldet51,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BG9" s="17">
+        <f>COUNTIFS(angemeldet52,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BH9" s="17">
+        <f>COUNTIFS(angemeldet53,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BI9" s="17">
+        <f>COUNTIFS(angemeldet54,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BJ9" s="17">
+        <f>COUNTIFS(angemeldet55,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BK9" s="17">
+        <f>COUNTIFS(angemeldet56,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BL9" s="17">
+        <f>COUNTIFS(angemeldet57,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BM9" s="17">
+        <f>COUNTIFS(angemeldet58,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BN9" s="17">
+        <f>COUNTIFS(angemeldet59,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BO9" s="17">
+        <f>COUNTIFS(angemeldet60,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BP9" s="17">
+        <f>COUNTIFS(angemeldet61,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BQ9" s="17">
+        <f>COUNTIFS(angemeldet62,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BR9" s="17">
+        <f>COUNTIFS(angemeldet63,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BS9" s="17">
+        <f>COUNTIFS(angemeldet64,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BT9" s="17">
+        <f>COUNTIFS(angemeldet65,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BU9" s="17">
+        <f>COUNTIFS(angemeldet66,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BV9" s="17">
+        <f>COUNTIFS(angemeldet67,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BW9" s="17">
+        <f>COUNTIFS(angemeldet68,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BX9" s="17">
+        <f>COUNTIFS(angemeldet69,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BY9" s="17">
+        <f>COUNTIFS(angemeldet70,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="BZ9" s="17">
+        <f>COUNTIFS(angemeldet71,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CA9" s="17">
+        <f>COUNTIFS(angemeldet72,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CB9" s="17">
+        <f>COUNTIFS(angemeldet73,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CC9" s="17">
+        <f>COUNTIFS(angemeldet74,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CD9" s="17">
+        <f>COUNTIFS(angemeldet75,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CE9" s="17">
+        <f>COUNTIFS(angemeldet76,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CF9" s="17">
+        <f>COUNTIFS(angemeldet77,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CG9" s="17">
+        <f>COUNTIFS(angemeldet78,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CH9" s="17">
+        <f>COUNTIFS(angemeldet79,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CI9" s="17">
+        <f>COUNTIFS(angemeldet80,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CJ9" s="17">
+        <f>COUNTIFS(angemeldet81,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CK9" s="17">
+        <f>COUNTIFS(angemeldet82,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CL9" s="17">
+        <f>COUNTIFS(angemeldet83,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CM9" s="17">
+        <f>COUNTIFS(angemeldet84,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CN9" s="17">
+        <f>COUNTIFS(angemeldet85,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CO9" s="17">
+        <f>COUNTIFS(angemeldet86,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CP9" s="17">
+        <f>COUNTIFS(angemeldet87,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CQ9" s="17">
+        <f>COUNTIFS(angemeldet88,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CR9" s="17">
+        <f>COUNTIFS(angemeldet89,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CS9" s="17">
+        <f>COUNTIFS(angemeldet90,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CT9" s="17">
+        <f>COUNTIFS(angemeldet91,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CU9" s="17">
+        <f>COUNTIFS(angemeldet92,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CV9" s="17">
+        <f>COUNTIFS(angemeldet93,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CW9" s="17">
+        <f>COUNTIFS(angemeldet94,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CX9" s="17">
+        <f>COUNTIFS(angemeldet95,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CY9" s="17">
+        <f>COUNTIFS(angemeldet96,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="CZ9" s="17">
+        <f>COUNTIFS(angemeldet97,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="DA9" s="17">
+        <f>COUNTIFS(angemeldet98,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="DB9" s="17">
+        <f>COUNTIFS(angemeldet99,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+      <c r="DC9" s="17">
+        <f>COUNTIFS(angemeldet100,"X",statusKategorie,$B$27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="17">
+        <f>COUNTIF(statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17">
+        <f>COUNTIFS(angemeldet1,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="17">
+        <f>COUNTIFS(angemeldet2,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="17">
+        <f>COUNTIFS(angemeldet3,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="17">
+        <f>COUNTIFS(angemeldet4,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="L10" s="17">
+        <f>COUNTIFS(angemeldet5,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="17">
+        <f>COUNTIFS(angemeldet6,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="17">
+        <f>COUNTIFS(angemeldet7,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="O10" s="17">
+        <f>COUNTIFS(angemeldet8,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="17">
+        <f>COUNTIFS(angemeldet9,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="17">
+        <f>COUNTIFS(angemeldet10,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="R10" s="17">
+        <f>COUNTIFS(angemeldet11,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="S10" s="17">
+        <f>COUNTIFS(angemeldet12,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="T10" s="17">
+        <f>COUNTIFS(angemeldet13,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="U10" s="17">
+        <f>COUNTIFS(angemeldet14,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="V10" s="17">
+        <f>COUNTIFS(angemeldet15,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="W10" s="17">
+        <f>COUNTIFS(angemeldet16,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="X10" s="17">
+        <f>COUNTIFS(angemeldet17,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="Y10" s="17">
+        <f>COUNTIFS(angemeldet18,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="Z10" s="17">
+        <f>COUNTIFS(angemeldet19,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AA10" s="17">
+        <f>COUNTIFS(angemeldet20,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AB10" s="17">
+        <f>COUNTIFS(angemeldet21,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AC10" s="17">
+        <f>COUNTIFS(angemeldet22,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AD10" s="17">
+        <f>COUNTIFS(angemeldet23,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AE10" s="17">
+        <f>COUNTIFS(angemeldet24,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AF10" s="17">
+        <f>COUNTIFS(angemeldet25,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AG10" s="17">
+        <f>COUNTIFS(angemeldet26,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AH10" s="17">
+        <f>COUNTIFS(angemeldet27,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AI10" s="17">
+        <f>COUNTIFS(angemeldet28,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="17">
+        <f>COUNTIFS(angemeldet29,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AK10" s="17">
+        <f>COUNTIFS(angemeldet30,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AL10" s="17">
+        <f>COUNTIFS(angemeldet31,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AM10" s="17">
+        <f>COUNTIFS(angemeldet32,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AN10" s="17">
+        <f>COUNTIFS(angemeldet33,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AO10" s="17">
+        <f>COUNTIFS(angemeldet34,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AP10" s="17">
+        <f>COUNTIFS(angemeldet35,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="17">
+        <f>COUNTIFS(angemeldet36,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AR10" s="17">
+        <f>COUNTIFS(angemeldet37,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AS10" s="17">
+        <f>COUNTIFS(angemeldet38,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AT10" s="17">
+        <f>COUNTIFS(angemeldet39,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AU10" s="17">
+        <f>COUNTIFS(angemeldet40,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AV10" s="17">
+        <f>COUNTIFS(angemeldet41,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AW10" s="17">
+        <f>COUNTIFS(angemeldet42,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AX10" s="17">
+        <f>COUNTIFS(angemeldet43,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AY10" s="17">
+        <f>COUNTIFS(angemeldet44,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="AZ10" s="17">
+        <f>COUNTIFS(angemeldet45,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BA10" s="17">
+        <f>COUNTIFS(angemeldet46,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BB10" s="17">
+        <f>COUNTIFS(angemeldet47,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BC10" s="17">
+        <f>COUNTIFS(angemeldet48,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BD10" s="17">
+        <f>COUNTIFS(angemeldet49,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BE10" s="17">
+        <f>COUNTIFS(angemeldet50,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BF10" s="17">
+        <f>COUNTIFS(angemeldet51,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BG10" s="17">
+        <f>COUNTIFS(angemeldet52,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BH10" s="17">
+        <f>COUNTIFS(angemeldet53,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BI10" s="17">
+        <f>COUNTIFS(angemeldet54,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BJ10" s="17">
+        <f>COUNTIFS(angemeldet55,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BK10" s="17">
+        <f>COUNTIFS(angemeldet56,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BL10" s="17">
+        <f>COUNTIFS(angemeldet57,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BM10" s="17">
+        <f>COUNTIFS(angemeldet58,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BN10" s="17">
+        <f>COUNTIFS(angemeldet59,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BO10" s="17">
+        <f>COUNTIFS(angemeldet60,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BP10" s="17">
+        <f>COUNTIFS(angemeldet61,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BQ10" s="17">
+        <f>COUNTIFS(angemeldet62,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BR10" s="17">
+        <f>COUNTIFS(angemeldet63,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BS10" s="17">
+        <f>COUNTIFS(angemeldet64,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BT10" s="17">
+        <f>COUNTIFS(angemeldet65,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BU10" s="17">
+        <f>COUNTIFS(angemeldet66,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BV10" s="17">
+        <f>COUNTIFS(angemeldet67,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BW10" s="17">
+        <f>COUNTIFS(angemeldet68,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BX10" s="17">
+        <f>COUNTIFS(angemeldet69,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BY10" s="17">
+        <f>COUNTIFS(angemeldet70,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="BZ10" s="17">
+        <f>COUNTIFS(angemeldet71,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CA10" s="17">
+        <f>COUNTIFS(angemeldet72,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CB10" s="17">
+        <f>COUNTIFS(angemeldet73,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CC10" s="17">
+        <f>COUNTIFS(angemeldet74,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CD10" s="17">
+        <f>COUNTIFS(angemeldet75,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CE10" s="17">
+        <f>COUNTIFS(angemeldet76,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CF10" s="17">
+        <f>COUNTIFS(angemeldet77,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CG10" s="17">
+        <f>COUNTIFS(angemeldet78,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CH10" s="17">
+        <f>COUNTIFS(angemeldet79,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CI10" s="17">
+        <f>COUNTIFS(angemeldet80,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CJ10" s="17">
+        <f>COUNTIFS(angemeldet81,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CK10" s="17">
+        <f>COUNTIFS(angemeldet82,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CL10" s="17">
+        <f>COUNTIFS(angemeldet83,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CM10" s="17">
+        <f>COUNTIFS(angemeldet84,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CN10" s="17">
+        <f>COUNTIFS(angemeldet85,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CO10" s="17">
+        <f>COUNTIFS(angemeldet86,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CP10" s="17">
+        <f>COUNTIFS(angemeldet87,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CQ10" s="17">
+        <f>COUNTIFS(angemeldet88,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CR10" s="17">
+        <f>COUNTIFS(angemeldet89,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CS10" s="17">
+        <f>COUNTIFS(angemeldet90,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CT10" s="17">
+        <f>COUNTIFS(angemeldet91,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CU10" s="17">
+        <f>COUNTIFS(angemeldet92,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CV10" s="17">
+        <f>COUNTIFS(angemeldet93,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CW10" s="17">
+        <f>COUNTIFS(angemeldet94,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CX10" s="17">
+        <f>COUNTIFS(angemeldet95,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CY10" s="17">
+        <f>COUNTIFS(angemeldet96,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="CZ10" s="17">
+        <f>COUNTIFS(angemeldet97,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="DA10" s="17">
+        <f>COUNTIFS(angemeldet98,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="DB10" s="17">
+        <f>COUNTIFS(angemeldet99,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+      <c r="DC10" s="17">
+        <f>COUNTIFS(angemeldet100,"X",statusKategorie,$B$26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:108" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19"/>
+      <c r="X11" s="19"/>
+      <c r="Y11" s="19"/>
+      <c r="Z11" s="19"/>
+      <c r="AA11" s="19"/>
+      <c r="AB11" s="19"/>
+      <c r="AC11" s="19"/>
+      <c r="AD11" s="19"/>
+      <c r="AE11" s="19"/>
+      <c r="AF11" s="19"/>
+      <c r="AG11" s="19"/>
+      <c r="AH11" s="19"/>
+      <c r="AI11" s="19"/>
+      <c r="AJ11" s="19"/>
+      <c r="AK11" s="19"/>
+      <c r="AL11" s="19"/>
+      <c r="AM11" s="19"/>
+      <c r="AN11" s="19"/>
+      <c r="AO11" s="19"/>
+      <c r="AP11" s="19"/>
+      <c r="AQ11" s="19"/>
+      <c r="AR11" s="19"/>
+      <c r="AS11" s="19"/>
+      <c r="AT11" s="19"/>
+      <c r="AU11" s="19"/>
+      <c r="AV11" s="19"/>
+      <c r="AW11" s="19"/>
+      <c r="AX11" s="19"/>
+      <c r="AY11" s="19"/>
+      <c r="AZ11" s="19"/>
+      <c r="BA11" s="19"/>
+      <c r="BB11" s="19"/>
+      <c r="BC11" s="19"/>
+      <c r="BD11" s="19"/>
+      <c r="BE11" s="19"/>
+      <c r="BF11" s="19"/>
+      <c r="BG11" s="19"/>
+      <c r="BH11" s="19"/>
+      <c r="BI11" s="19"/>
+      <c r="BJ11" s="19"/>
+      <c r="BK11" s="19"/>
+      <c r="BL11" s="19"/>
+      <c r="BM11" s="19"/>
+      <c r="BN11" s="19"/>
+      <c r="BO11" s="19"/>
+      <c r="BP11" s="19"/>
+      <c r="BQ11" s="19"/>
+      <c r="BR11" s="19"/>
+      <c r="BS11" s="19"/>
+      <c r="BT11" s="19"/>
+      <c r="BU11" s="19"/>
+      <c r="BV11" s="19"/>
+      <c r="BW11" s="19"/>
+      <c r="BX11" s="19"/>
+      <c r="BY11" s="19"/>
+      <c r="BZ11" s="19"/>
+      <c r="CA11" s="19"/>
+      <c r="CB11" s="19"/>
+      <c r="CC11" s="19"/>
+      <c r="CD11" s="19"/>
+      <c r="CE11" s="19"/>
+      <c r="CF11" s="19"/>
+      <c r="CG11" s="19"/>
+      <c r="CH11" s="19"/>
+      <c r="CI11" s="19"/>
+      <c r="CJ11" s="19"/>
+      <c r="CK11" s="19"/>
+      <c r="CL11" s="19"/>
+      <c r="CM11" s="19"/>
+      <c r="CN11" s="19"/>
+      <c r="CO11" s="19"/>
+      <c r="CP11" s="19"/>
+      <c r="CQ11" s="19"/>
+      <c r="CR11" s="19"/>
+      <c r="CS11" s="19"/>
+      <c r="CT11" s="19"/>
+      <c r="CU11" s="19"/>
+      <c r="CV11" s="19"/>
+      <c r="CW11" s="19"/>
+      <c r="CX11" s="19"/>
+      <c r="CY11" s="19"/>
+      <c r="CZ11" s="19"/>
+      <c r="DA11" s="19"/>
+      <c r="DB11" s="19"/>
+      <c r="DC11" s="19"/>
+    </row>
+    <row r="13" spans="1:108" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="str">
+        <f>B26</f>
+        <v>OFFEN</v>
+      </c>
+    </row>
+    <row r="14" spans="1:108" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="str">
+        <f>B26</f>
+        <v>OFFEN</v>
+      </c>
+    </row>
+    <row r="15" spans="1:108" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="str">
+        <f>B28</f>
+        <v>BESTÄTIGT</v>
+      </c>
+    </row>
+    <row r="16" spans="1:108" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="str">
+        <f>B27</f>
+        <v>ABGELEHNT</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="str">
+        <f>B26</f>
+        <v>OFFEN</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="str">
+        <f>B28</f>
+        <v>BESTÄTIGT</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="str">
+        <f>B26</f>
+        <v>OFFEN</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="str">
+        <f>B26</f>
+        <v>OFFEN</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="str">
+        <f>B28</f>
+        <v>BESTÄTIGT</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="str">
+        <f>B27</f>
+        <v>ABGELEHNT</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="str">
+        <f>B26</f>
+        <v>OFFEN</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="str">
+        <f>B28</f>
+        <v>BESTÄTIGT</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="G5:Z5"/>
-    <mergeCell ref="AA5:AT5"/>
-    <mergeCell ref="AU5:BN5"/>
-    <mergeCell ref="BO5:CH5"/>
-    <mergeCell ref="CI5:DB5"/>
+  <mergeCells count="9">
+    <mergeCell ref="AV5:BO5"/>
+    <mergeCell ref="BP5:CI5"/>
+    <mergeCell ref="CJ5:DC5"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A8:E8"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="H5:AA5"/>
+    <mergeCell ref="AB5:AU5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-1218 Wochentage statisch statt dynamisch einfüllen um Fehler zu vermeiden
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/TagesschuleOhneFinSit.xlsx
+++ b/ebegu-server/src/main/resources/reporting/TagesschuleOhneFinSit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0523F2E8-CAE6-46C6-9D3F-2EA67B212B1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C87685-14CB-43C5-B2EA-2FFF843E248C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="50">
   <si>
     <t>{statusTitle}</t>
   </si>
@@ -180,9 +180,6 @@
     <t>{angemeldet}</t>
   </si>
   <si>
-    <t>{wochentag}</t>
-  </si>
-  <si>
     <t>{periode}</t>
   </si>
   <si>
@@ -274,6 +271,21 @@
   </si>
   <si>
     <t>{nichtFreigegebenAnzahl}</t>
+  </si>
+  <si>
+    <t>{wochentagDi}</t>
+  </si>
+  <si>
+    <t>{wochentagMo}</t>
+  </si>
+  <si>
+    <t>{wochentagMi}</t>
+  </si>
+  <si>
+    <t>{wochentagDo}</t>
+  </si>
+  <si>
+    <t>{wochentagFr}</t>
   </si>
 </sst>
 </file>
@@ -890,9 +902,7 @@
   </sheetPr>
   <dimension ref="A1:DD28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -926,7 +936,7 @@
     </row>
     <row r="2" spans="1:108" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
@@ -1052,304 +1062,304 @@
     <row r="4" spans="1:108" x14ac:dyDescent="0.25">
       <c r="C4"/>
       <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>17</v>
+      </c>
+      <c r="R4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S4" t="s">
+        <v>17</v>
+      </c>
+      <c r="T4" t="s">
+        <v>17</v>
+      </c>
+      <c r="U4" t="s">
+        <v>17</v>
+      </c>
+      <c r="V4" t="s">
+        <v>17</v>
+      </c>
+      <c r="W4" t="s">
+        <v>17</v>
+      </c>
+      <c r="X4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB4" t="s">
         <v>18</v>
       </c>
-      <c r="I4" t="s">
+      <c r="AC4" t="s">
         <v>18</v>
       </c>
-      <c r="J4" t="s">
+      <c r="AD4" t="s">
         <v>18</v>
       </c>
-      <c r="K4" t="s">
+      <c r="AE4" t="s">
         <v>18</v>
       </c>
-      <c r="L4" t="s">
+      <c r="AF4" t="s">
         <v>18</v>
       </c>
-      <c r="M4" t="s">
+      <c r="AG4" t="s">
         <v>18</v>
       </c>
-      <c r="N4" t="s">
+      <c r="AH4" t="s">
         <v>18</v>
       </c>
-      <c r="O4" t="s">
+      <c r="AI4" t="s">
         <v>18</v>
       </c>
-      <c r="P4" t="s">
+      <c r="AJ4" t="s">
         <v>18</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="AK4" t="s">
         <v>18</v>
       </c>
-      <c r="R4" t="s">
+      <c r="AL4" t="s">
         <v>18</v>
       </c>
-      <c r="S4" t="s">
+      <c r="AM4" t="s">
         <v>18</v>
       </c>
-      <c r="T4" t="s">
+      <c r="AN4" t="s">
         <v>18</v>
       </c>
-      <c r="U4" t="s">
+      <c r="AO4" t="s">
         <v>18</v>
       </c>
-      <c r="V4" t="s">
+      <c r="AP4" t="s">
         <v>18</v>
       </c>
-      <c r="W4" t="s">
+      <c r="AQ4" t="s">
         <v>18</v>
       </c>
-      <c r="X4" t="s">
+      <c r="AR4" t="s">
         <v>18</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AS4" t="s">
         <v>18</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AT4" t="s">
         <v>18</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AU4" t="s">
         <v>18</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AV4" t="s">
         <v>19</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AW4" t="s">
         <v>19</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AX4" t="s">
         <v>19</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AY4" t="s">
         <v>19</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AZ4" t="s">
         <v>19</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="BA4" t="s">
         <v>19</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="BB4" t="s">
         <v>19</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="BC4" t="s">
         <v>19</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="BD4" t="s">
         <v>19</v>
       </c>
-      <c r="AK4" t="s">
+      <c r="BE4" t="s">
         <v>19</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="BF4" t="s">
         <v>19</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="BG4" t="s">
         <v>19</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="BH4" t="s">
         <v>19</v>
       </c>
-      <c r="AO4" t="s">
+      <c r="BI4" t="s">
         <v>19</v>
       </c>
-      <c r="AP4" t="s">
+      <c r="BJ4" t="s">
         <v>19</v>
       </c>
-      <c r="AQ4" t="s">
+      <c r="BK4" t="s">
         <v>19</v>
       </c>
-      <c r="AR4" t="s">
+      <c r="BL4" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" t="s">
+      <c r="BM4" t="s">
         <v>19</v>
       </c>
-      <c r="AT4" t="s">
+      <c r="BN4" t="s">
         <v>19</v>
       </c>
-      <c r="AU4" t="s">
+      <c r="BO4" t="s">
         <v>19</v>
       </c>
-      <c r="AV4" t="s">
+      <c r="BP4" t="s">
         <v>20</v>
       </c>
-      <c r="AW4" t="s">
+      <c r="BQ4" t="s">
         <v>20</v>
       </c>
-      <c r="AX4" t="s">
+      <c r="BR4" t="s">
         <v>20</v>
       </c>
-      <c r="AY4" t="s">
+      <c r="BS4" t="s">
         <v>20</v>
       </c>
-      <c r="AZ4" t="s">
+      <c r="BT4" t="s">
         <v>20</v>
       </c>
-      <c r="BA4" t="s">
+      <c r="BU4" t="s">
         <v>20</v>
       </c>
-      <c r="BB4" t="s">
+      <c r="BV4" t="s">
         <v>20</v>
       </c>
-      <c r="BC4" t="s">
+      <c r="BW4" t="s">
         <v>20</v>
       </c>
-      <c r="BD4" t="s">
+      <c r="BX4" t="s">
         <v>20</v>
       </c>
-      <c r="BE4" t="s">
+      <c r="BY4" t="s">
         <v>20</v>
       </c>
-      <c r="BF4" t="s">
+      <c r="BZ4" t="s">
         <v>20</v>
       </c>
-      <c r="BG4" t="s">
+      <c r="CA4" t="s">
         <v>20</v>
       </c>
-      <c r="BH4" t="s">
+      <c r="CB4" t="s">
         <v>20</v>
       </c>
-      <c r="BI4" t="s">
+      <c r="CC4" t="s">
         <v>20</v>
       </c>
-      <c r="BJ4" t="s">
+      <c r="CD4" t="s">
         <v>20</v>
       </c>
-      <c r="BK4" t="s">
+      <c r="CE4" t="s">
         <v>20</v>
       </c>
-      <c r="BL4" t="s">
+      <c r="CF4" t="s">
         <v>20</v>
       </c>
-      <c r="BM4" t="s">
+      <c r="CG4" t="s">
         <v>20</v>
       </c>
-      <c r="BN4" t="s">
+      <c r="CH4" t="s">
         <v>20</v>
       </c>
-      <c r="BO4" t="s">
+      <c r="CI4" t="s">
         <v>20</v>
       </c>
-      <c r="BP4" t="s">
+      <c r="CJ4" t="s">
         <v>21</v>
       </c>
-      <c r="BQ4" t="s">
+      <c r="CK4" t="s">
         <v>21</v>
       </c>
-      <c r="BR4" t="s">
+      <c r="CL4" t="s">
         <v>21</v>
       </c>
-      <c r="BS4" t="s">
+      <c r="CM4" t="s">
         <v>21</v>
       </c>
-      <c r="BT4" t="s">
+      <c r="CN4" t="s">
         <v>21</v>
       </c>
-      <c r="BU4" t="s">
+      <c r="CO4" t="s">
         <v>21</v>
       </c>
-      <c r="BV4" t="s">
+      <c r="CP4" t="s">
         <v>21</v>
       </c>
-      <c r="BW4" t="s">
+      <c r="CQ4" t="s">
         <v>21</v>
       </c>
-      <c r="BX4" t="s">
+      <c r="CR4" t="s">
         <v>21</v>
       </c>
-      <c r="BY4" t="s">
+      <c r="CS4" t="s">
         <v>21</v>
       </c>
-      <c r="BZ4" t="s">
+      <c r="CT4" t="s">
         <v>21</v>
       </c>
-      <c r="CA4" t="s">
+      <c r="CU4" t="s">
         <v>21</v>
       </c>
-      <c r="CB4" t="s">
+      <c r="CV4" t="s">
         <v>21</v>
       </c>
-      <c r="CC4" t="s">
+      <c r="CW4" t="s">
         <v>21</v>
       </c>
-      <c r="CD4" t="s">
+      <c r="CX4" t="s">
         <v>21</v>
       </c>
-      <c r="CE4" t="s">
+      <c r="CY4" t="s">
         <v>21</v>
       </c>
-      <c r="CF4" t="s">
+      <c r="CZ4" t="s">
         <v>21</v>
       </c>
-      <c r="CG4" t="s">
+      <c r="DA4" t="s">
         <v>21</v>
       </c>
-      <c r="CH4" t="s">
+      <c r="DB4" t="s">
         <v>21</v>
       </c>
-      <c r="CI4" t="s">
+      <c r="DC4" t="s">
         <v>21</v>
-      </c>
-      <c r="CJ4" t="s">
-        <v>22</v>
-      </c>
-      <c r="CK4" t="s">
-        <v>22</v>
-      </c>
-      <c r="CL4" t="s">
-        <v>22</v>
-      </c>
-      <c r="CM4" t="s">
-        <v>22</v>
-      </c>
-      <c r="CN4" t="s">
-        <v>22</v>
-      </c>
-      <c r="CO4" t="s">
-        <v>22</v>
-      </c>
-      <c r="CP4" t="s">
-        <v>22</v>
-      </c>
-      <c r="CQ4" t="s">
-        <v>22</v>
-      </c>
-      <c r="CR4" t="s">
-        <v>22</v>
-      </c>
-      <c r="CS4" t="s">
-        <v>22</v>
-      </c>
-      <c r="CT4" t="s">
-        <v>22</v>
-      </c>
-      <c r="CU4" t="s">
-        <v>22</v>
-      </c>
-      <c r="CV4" t="s">
-        <v>22</v>
-      </c>
-      <c r="CW4" t="s">
-        <v>22</v>
-      </c>
-      <c r="CX4" t="s">
-        <v>22</v>
-      </c>
-      <c r="CY4" t="s">
-        <v>22</v>
-      </c>
-      <c r="CZ4" t="s">
-        <v>22</v>
-      </c>
-      <c r="DA4" t="s">
-        <v>22</v>
-      </c>
-      <c r="DB4" t="s">
-        <v>22</v>
-      </c>
-      <c r="DC4" t="s">
-        <v>22</v>
       </c>
       <c r="DD4" s="14"/>
     </row>
@@ -1361,7 +1371,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>9</v>
@@ -1374,7 +1384,7 @@
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="20" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="I5" s="21"/>
       <c r="J5" s="21"/>
@@ -1396,7 +1406,7 @@
       <c r="Z5" s="21"/>
       <c r="AA5" s="22"/>
       <c r="AB5" s="20" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="AC5" s="21"/>
       <c r="AD5" s="21"/>
@@ -1418,7 +1428,7 @@
       <c r="AT5" s="21"/>
       <c r="AU5" s="22"/>
       <c r="AV5" s="20" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="AW5" s="21"/>
       <c r="AX5" s="21"/>
@@ -1440,7 +1450,7 @@
       <c r="BN5" s="21"/>
       <c r="BO5" s="22"/>
       <c r="BP5" s="20" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="BQ5" s="21"/>
       <c r="BR5" s="21"/>
@@ -1462,7 +1472,7 @@
       <c r="CH5" s="21"/>
       <c r="CI5" s="22"/>
       <c r="CJ5" s="20" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="CK5" s="21"/>
       <c r="CL5" s="21"/>
@@ -1482,7 +1492,7 @@
       <c r="CZ5" s="21"/>
       <c r="DA5" s="21"/>
       <c r="DB5" s="21"/>
-      <c r="DC5" s="21"/>
+      <c r="DC5" s="22"/>
       <c r="DD5" s="12"/>
     </row>
     <row r="6" spans="1:108" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2119,12 +2129,12 @@
         <v>13</v>
       </c>
       <c r="DD7" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A8" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="25"/>
       <c r="C8" s="25"/>
@@ -2538,7 +2548,7 @@
     </row>
     <row r="9" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="25"/>
@@ -2952,7 +2962,7 @@
     </row>
     <row r="10" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="25"/>
@@ -3366,14 +3376,14 @@
     </row>
     <row r="11" spans="1:108" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
       <c r="F11" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
@@ -3478,7 +3488,7 @@
     </row>
     <row r="13" spans="1:108" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" t="str">
         <f>B26</f>
@@ -3487,7 +3497,7 @@
     </row>
     <row r="14" spans="1:108" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" t="str">
         <f>B26</f>
@@ -3496,7 +3506,7 @@
     </row>
     <row r="15" spans="1:108" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" t="str">
         <f>B28</f>
@@ -3505,7 +3515,7 @@
     </row>
     <row r="16" spans="1:108" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" t="str">
         <f>B27</f>
@@ -3514,7 +3524,7 @@
     </row>
     <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" t="str">
         <f>B26</f>
@@ -3523,7 +3533,7 @@
     </row>
     <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" t="str">
         <f>B28</f>
@@ -3532,7 +3542,7 @@
     </row>
     <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" t="str">
         <f>B26</f>
@@ -3541,7 +3551,7 @@
     </row>
     <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" t="str">
         <f>B26</f>
@@ -3550,7 +3560,7 @@
     </row>
     <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" t="str">
         <f>B28</f>
@@ -3559,7 +3569,7 @@
     </row>
     <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" t="str">
         <f>B27</f>
@@ -3568,7 +3578,7 @@
     </row>
     <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" t="str">
         <f>B26</f>
@@ -3577,7 +3587,7 @@
     </row>
     <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" t="str">
         <f>B28</f>
@@ -3587,26 +3597,26 @@
     <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s">
         <v>38</v>
-      </c>
-      <c r="B26" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" t="s">
         <v>40</v>
-      </c>
-      <c r="B27" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" t="s">
         <v>42</v>
-      </c>
-      <c r="B28" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
direct-to-dev: Tagesschule Statistik angepasst
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/TagesschuleOhneFinSit.xlsx
+++ b/ebegu-server/src/main/resources/reporting/TagesschuleOhneFinSit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12E02E9-62DD-4E23-826E-6338F07B7BB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D0AB79-0381-44F6-807F-EC72BB6263B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,6 +117,7 @@
     <definedName name="angemeldet97">Data!$CZ$7</definedName>
     <definedName name="angemeldet98">Data!$DA$7</definedName>
     <definedName name="angemeldet99">Data!$DB$7</definedName>
+    <definedName name="freigegebenKategorie">Data!$G$11</definedName>
     <definedName name="nichtFreigegeben1">Data!$H$11</definedName>
     <definedName name="nichtFreigegeben10">Data!$Q$11</definedName>
     <definedName name="nichtFreigegeben100">Data!$DC$11</definedName>
@@ -598,6 +599,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -607,6 +609,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -616,8 +619,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1491,144 +1492,144 @@
       <c r="DD4" s="13"/>
     </row>
     <row r="5" spans="1:108" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F5" s="26" t="s">
         <v>0</v>
       </c>
       <c r="G5" s="16"/>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
-      <c r="S5" s="19"/>
-      <c r="T5" s="19"/>
-      <c r="U5" s="19"/>
-      <c r="V5" s="19"/>
-      <c r="W5" s="19"/>
-      <c r="X5" s="19"/>
-      <c r="Y5" s="19"/>
-      <c r="Z5" s="19"/>
-      <c r="AA5" s="20"/>
-      <c r="AB5" s="18" t="s">
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="20"/>
+      <c r="W5" s="20"/>
+      <c r="X5" s="20"/>
+      <c r="Y5" s="20"/>
+      <c r="Z5" s="20"/>
+      <c r="AA5" s="21"/>
+      <c r="AB5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="AC5" s="19"/>
-      <c r="AD5" s="19"/>
-      <c r="AE5" s="19"/>
-      <c r="AF5" s="19"/>
-      <c r="AG5" s="19"/>
-      <c r="AH5" s="19"/>
-      <c r="AI5" s="19"/>
-      <c r="AJ5" s="19"/>
-      <c r="AK5" s="19"/>
-      <c r="AL5" s="19"/>
-      <c r="AM5" s="19"/>
-      <c r="AN5" s="19"/>
-      <c r="AO5" s="19"/>
-      <c r="AP5" s="19"/>
-      <c r="AQ5" s="19"/>
-      <c r="AR5" s="19"/>
-      <c r="AS5" s="19"/>
-      <c r="AT5" s="19"/>
-      <c r="AU5" s="20"/>
-      <c r="AV5" s="18" t="s">
+      <c r="AC5" s="20"/>
+      <c r="AD5" s="20"/>
+      <c r="AE5" s="20"/>
+      <c r="AF5" s="20"/>
+      <c r="AG5" s="20"/>
+      <c r="AH5" s="20"/>
+      <c r="AI5" s="20"/>
+      <c r="AJ5" s="20"/>
+      <c r="AK5" s="20"/>
+      <c r="AL5" s="20"/>
+      <c r="AM5" s="20"/>
+      <c r="AN5" s="20"/>
+      <c r="AO5" s="20"/>
+      <c r="AP5" s="20"/>
+      <c r="AQ5" s="20"/>
+      <c r="AR5" s="20"/>
+      <c r="AS5" s="20"/>
+      <c r="AT5" s="20"/>
+      <c r="AU5" s="21"/>
+      <c r="AV5" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="AW5" s="19"/>
-      <c r="AX5" s="19"/>
-      <c r="AY5" s="19"/>
-      <c r="AZ5" s="19"/>
-      <c r="BA5" s="19"/>
-      <c r="BB5" s="19"/>
-      <c r="BC5" s="19"/>
-      <c r="BD5" s="19"/>
-      <c r="BE5" s="19"/>
-      <c r="BF5" s="19"/>
-      <c r="BG5" s="19"/>
-      <c r="BH5" s="19"/>
-      <c r="BI5" s="19"/>
-      <c r="BJ5" s="19"/>
-      <c r="BK5" s="19"/>
-      <c r="BL5" s="19"/>
-      <c r="BM5" s="19"/>
-      <c r="BN5" s="19"/>
-      <c r="BO5" s="20"/>
-      <c r="BP5" s="18" t="s">
+      <c r="AW5" s="20"/>
+      <c r="AX5" s="20"/>
+      <c r="AY5" s="20"/>
+      <c r="AZ5" s="20"/>
+      <c r="BA5" s="20"/>
+      <c r="BB5" s="20"/>
+      <c r="BC5" s="20"/>
+      <c r="BD5" s="20"/>
+      <c r="BE5" s="20"/>
+      <c r="BF5" s="20"/>
+      <c r="BG5" s="20"/>
+      <c r="BH5" s="20"/>
+      <c r="BI5" s="20"/>
+      <c r="BJ5" s="20"/>
+      <c r="BK5" s="20"/>
+      <c r="BL5" s="20"/>
+      <c r="BM5" s="20"/>
+      <c r="BN5" s="20"/>
+      <c r="BO5" s="21"/>
+      <c r="BP5" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="BQ5" s="19"/>
-      <c r="BR5" s="19"/>
-      <c r="BS5" s="19"/>
-      <c r="BT5" s="19"/>
-      <c r="BU5" s="19"/>
-      <c r="BV5" s="19"/>
-      <c r="BW5" s="19"/>
-      <c r="BX5" s="19"/>
-      <c r="BY5" s="19"/>
-      <c r="BZ5" s="19"/>
-      <c r="CA5" s="19"/>
-      <c r="CB5" s="19"/>
-      <c r="CC5" s="19"/>
-      <c r="CD5" s="19"/>
-      <c r="CE5" s="19"/>
-      <c r="CF5" s="19"/>
-      <c r="CG5" s="19"/>
-      <c r="CH5" s="19"/>
-      <c r="CI5" s="20"/>
-      <c r="CJ5" s="18" t="s">
+      <c r="BQ5" s="20"/>
+      <c r="BR5" s="20"/>
+      <c r="BS5" s="20"/>
+      <c r="BT5" s="20"/>
+      <c r="BU5" s="20"/>
+      <c r="BV5" s="20"/>
+      <c r="BW5" s="20"/>
+      <c r="BX5" s="20"/>
+      <c r="BY5" s="20"/>
+      <c r="BZ5" s="20"/>
+      <c r="CA5" s="20"/>
+      <c r="CB5" s="20"/>
+      <c r="CC5" s="20"/>
+      <c r="CD5" s="20"/>
+      <c r="CE5" s="20"/>
+      <c r="CF5" s="20"/>
+      <c r="CG5" s="20"/>
+      <c r="CH5" s="20"/>
+      <c r="CI5" s="21"/>
+      <c r="CJ5" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="CK5" s="19"/>
-      <c r="CL5" s="19"/>
-      <c r="CM5" s="19"/>
-      <c r="CN5" s="19"/>
-      <c r="CO5" s="19"/>
-      <c r="CP5" s="19"/>
-      <c r="CQ5" s="19"/>
-      <c r="CR5" s="19"/>
-      <c r="CS5" s="19"/>
-      <c r="CT5" s="19"/>
-      <c r="CU5" s="19"/>
-      <c r="CV5" s="19"/>
-      <c r="CW5" s="19"/>
-      <c r="CX5" s="19"/>
-      <c r="CY5" s="19"/>
-      <c r="CZ5" s="19"/>
-      <c r="DA5" s="19"/>
-      <c r="DB5" s="19"/>
-      <c r="DC5" s="20"/>
+      <c r="CK5" s="20"/>
+      <c r="CL5" s="20"/>
+      <c r="CM5" s="20"/>
+      <c r="CN5" s="20"/>
+      <c r="CO5" s="20"/>
+      <c r="CP5" s="20"/>
+      <c r="CQ5" s="20"/>
+      <c r="CR5" s="20"/>
+      <c r="CS5" s="20"/>
+      <c r="CT5" s="20"/>
+      <c r="CU5" s="20"/>
+      <c r="CV5" s="20"/>
+      <c r="CW5" s="20"/>
+      <c r="CX5" s="20"/>
+      <c r="CY5" s="20"/>
+      <c r="CZ5" s="20"/>
+      <c r="DA5" s="20"/>
+      <c r="DB5" s="20"/>
+      <c r="DC5" s="21"/>
       <c r="DD5" s="11"/>
     </row>
     <row r="6" spans="1:108" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
       <c r="G6" s="17"/>
       <c r="H6" s="4" t="s">
         <v>7</v>
@@ -2260,13 +2261,13 @@
       </c>
     </row>
     <row r="8" spans="1:108" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25"/>
       <c r="F8" s="15">
         <f>COUNTIF(statusKategorie,$B$29)</f>
         <v>0</v>
@@ -2674,13 +2675,13 @@
       </c>
     </row>
     <row r="9" spans="1:108" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25"/>
       <c r="F9" s="15">
         <f>COUNTIF(statusKategorie,$B$28)</f>
         <v>0</v>
@@ -3088,416 +3089,416 @@
       </c>
     </row>
     <row r="10" spans="1:108" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="23"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
       <c r="F10" s="15">
         <f>COUNTIF(statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="15">
-        <f>COUNTIF(angemeldet1,"X")</f>
+        <f>COUNTIFS(angemeldet1,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="I10" s="15">
-        <f>COUNTIF(angemeldet2,"X")</f>
+        <f>COUNTIFS(angemeldet2,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="J10" s="15">
-        <f>COUNTIF(angemeldet3,"X")</f>
+        <f>COUNTIFS(angemeldet3,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="K10" s="15">
-        <f>COUNTIF(angemeldet4,"X")</f>
+        <f>COUNTIFS(angemeldet4,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="L10" s="15">
-        <f>COUNTIF(angemeldet5,"X")</f>
+        <f>COUNTIFS(angemeldet5,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="M10" s="15">
-        <f>COUNTIF(angemeldet6,"X")</f>
+        <f>COUNTIFS(angemeldet6,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="N10" s="15">
-        <f>COUNTIF(angemeldet7,"X")</f>
+        <f>COUNTIFS(angemeldet7,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="O10" s="15">
-        <f>COUNTIF(angemeldet8,"X")</f>
+        <f>COUNTIFS(angemeldet8,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="P10" s="15">
-        <f>COUNTIF(angemeldet9,"X")</f>
+        <f>COUNTIFS(angemeldet9,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="Q10" s="15">
-        <f>COUNTIF(angemeldet10,"X")</f>
+        <f>COUNTIFS(angemeldet10,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="R10" s="15">
-        <f>COUNTIF(angemeldet11,"X")</f>
+        <f>COUNTIFS(angemeldet11,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="S10" s="15">
-        <f>COUNTIF(angemeldet12,"X")</f>
+        <f>COUNTIFS(angemeldet12,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="T10" s="15">
-        <f>COUNTIF(angemeldet13,"X")</f>
+        <f>COUNTIFS(angemeldet13,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="U10" s="15">
-        <f>COUNTIF(angemeldet14,"X")</f>
+        <f>COUNTIFS(angemeldet14,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="V10" s="15">
-        <f>COUNTIF(angemeldet15,"X")</f>
+        <f>COUNTIFS(angemeldet15,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="W10" s="15">
-        <f>COUNTIF(angemeldet16,"X")</f>
+        <f>COUNTIFS(angemeldet16,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="X10" s="15">
-        <f>COUNTIF(angemeldet17,"X")</f>
+        <f>COUNTIFS(angemeldet17,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="Y10" s="15">
-        <f>COUNTIF(angemeldet18,"X")</f>
+        <f>COUNTIFS(angemeldet18,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="Z10" s="15">
-        <f>COUNTIF(angemeldet19,"X")</f>
+        <f>COUNTIFS(angemeldet19,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AA10" s="15">
-        <f>COUNTIF(angemeldet20,"X")</f>
+        <f>COUNTIFS(angemeldet20,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AB10" s="15">
-        <f>COUNTIF(angemeldet21,"X")</f>
+        <f>COUNTIFS(angemeldet21,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AC10" s="15">
-        <f>COUNTIF(angemeldet22,"X")</f>
+        <f>COUNTIFS(angemeldet22,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AD10" s="15">
-        <f>COUNTIF(angemeldet23,"X")</f>
+        <f>COUNTIFS(angemeldet23,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AE10" s="15">
-        <f>COUNTIF(angemeldet24,"X")</f>
+        <f>COUNTIFS(angemeldet24,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AF10" s="15">
-        <f>COUNTIF(angemeldet25,"X")</f>
+        <f>COUNTIFS(angemeldet25,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AG10" s="15">
-        <f>COUNTIF(angemeldet26,"X")</f>
+        <f>COUNTIFS(angemeldet26,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AH10" s="15">
-        <f>COUNTIF(angemeldet27,"X")</f>
+        <f>COUNTIFS(angemeldet27,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AI10" s="15">
-        <f>COUNTIF(angemeldet28,"X")</f>
+        <f>COUNTIFS(angemeldet28,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AJ10" s="15">
-        <f>COUNTIF(angemeldet29,"X")</f>
+        <f>COUNTIFS(angemeldet29,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AK10" s="15">
-        <f>COUNTIF(angemeldet30,"X")</f>
+        <f>COUNTIFS(angemeldet30,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AL10" s="15">
-        <f>COUNTIF(angemeldet31,"X")</f>
+        <f>COUNTIFS(angemeldet31,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AM10" s="15">
-        <f>COUNTIF(angemeldet32,"X")</f>
+        <f>COUNTIFS(angemeldet32,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AN10" s="15">
-        <f>COUNTIF(angemeldet33,"X")</f>
+        <f>COUNTIFS(angemeldet33,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AO10" s="15">
-        <f>COUNTIF(angemeldet34,"X")</f>
+        <f>COUNTIFS(angemeldet34,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AP10" s="15">
-        <f>COUNTIF(angemeldet35,"X")</f>
+        <f>COUNTIFS(angemeldet35,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AQ10" s="15">
-        <f>COUNTIF(angemeldet36,"X")</f>
+        <f>COUNTIFS(angemeldet36,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AR10" s="15">
-        <f>COUNTIF(angemeldet37,"X")</f>
+        <f>COUNTIFS(angemeldet37,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AS10" s="15">
-        <f>COUNTIF(angemeldet38,"X")</f>
+        <f>COUNTIFS(angemeldet38,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AT10" s="15">
-        <f>COUNTIF(angemeldet39,"X")</f>
+        <f>COUNTIFS(angemeldet39,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AU10" s="15">
-        <f>COUNTIF(angemeldet40,"X")</f>
+        <f>COUNTIFS(angemeldet40,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AV10" s="15">
-        <f>COUNTIF(angemeldet41,"X")</f>
+        <f>COUNTIFS(angemeldet41,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AW10" s="15">
-        <f>COUNTIF(angemeldet42,"X")</f>
+        <f>COUNTIFS(angemeldet42,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AX10" s="15">
-        <f>COUNTIF(angemeldet43,"X")</f>
+        <f>COUNTIFS(angemeldet43,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AY10" s="15">
-        <f>COUNTIF(angemeldet44,"X")</f>
+        <f>COUNTIFS(angemeldet44,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="AZ10" s="15">
-        <f>COUNTIF(angemeldet45,"X")</f>
+        <f>COUNTIFS(angemeldet45,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BA10" s="15">
-        <f>COUNTIF(angemeldet46,"X")</f>
+        <f>COUNTIFS(angemeldet46,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BB10" s="15">
-        <f>COUNTIF(angemeldet47,"X")</f>
+        <f>COUNTIFS(angemeldet47,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BC10" s="15">
-        <f>COUNTIF(angemeldet48,"X")</f>
+        <f>COUNTIFS(angemeldet48,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BD10" s="15">
-        <f>COUNTIF(angemeldet49,"X")</f>
+        <f>COUNTIFS(angemeldet49,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BE10" s="15">
-        <f>COUNTIF(angemeldet50,"X")</f>
+        <f>COUNTIFS(angemeldet50,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BF10" s="15">
-        <f>COUNTIF(angemeldet51,"X")</f>
+        <f>COUNTIFS(angemeldet51,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BG10" s="15">
-        <f>COUNTIF(angemeldet52,"X")</f>
+        <f>COUNTIFS(angemeldet52,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BH10" s="15">
-        <f>COUNTIF(angemeldet53,"X")</f>
+        <f>COUNTIFS(angemeldet53,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BI10" s="15">
-        <f>COUNTIF(angemeldet54,"X")</f>
+        <f>COUNTIFS(angemeldet54,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BJ10" s="15">
-        <f>COUNTIF(angemeldet55,"X")</f>
+        <f>COUNTIFS(angemeldet55,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BK10" s="15">
-        <f>COUNTIF(angemeldet56,"X")</f>
+        <f>COUNTIFS(angemeldet56,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BL10" s="15">
-        <f>COUNTIF(angemeldet57,"X")</f>
+        <f>COUNTIFS(angemeldet57,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BM10" s="15">
-        <f>COUNTIF(angemeldet58,"X")</f>
+        <f>COUNTIFS(angemeldet58,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BN10" s="15">
-        <f>COUNTIF(angemeldet59,"X")</f>
+        <f>COUNTIFS(angemeldet59,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BO10" s="15">
-        <f>COUNTIF(angemeldet60,"X")</f>
+        <f>COUNTIFS(angemeldet60,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BP10" s="15">
-        <f>COUNTIF(angemeldet61,"X")</f>
+        <f>COUNTIFS(angemeldet61,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BQ10" s="15">
-        <f>COUNTIF(angemeldet62,"X")</f>
+        <f>COUNTIFS(angemeldet62,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BR10" s="15">
-        <f>COUNTIF(angemeldet63,"X")</f>
+        <f>COUNTIFS(angemeldet63,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BS10" s="15">
-        <f>COUNTIF(angemeldet64,"X")</f>
+        <f>COUNTIFS(angemeldet64,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BT10" s="15">
-        <f>COUNTIF(angemeldet65,"X")</f>
+        <f>COUNTIFS(angemeldet65,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BU10" s="15">
-        <f>COUNTIF(angemeldet66,"X")</f>
+        <f>COUNTIFS(angemeldet66,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BV10" s="15">
-        <f>COUNTIF(angemeldet67,"X")</f>
+        <f>COUNTIFS(angemeldet67,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BW10" s="15">
-        <f>COUNTIF(angemeldet68,"X")</f>
+        <f>COUNTIFS(angemeldet68,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BX10" s="15">
-        <f>COUNTIF(angemeldet69,"X")</f>
+        <f>COUNTIFS(angemeldet69,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BY10" s="15">
-        <f>COUNTIF(angemeldet70,"X")</f>
+        <f>COUNTIFS(angemeldet70,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="BZ10" s="15">
-        <f>COUNTIF(angemeldet71,"X")</f>
+        <f>COUNTIFS(angemeldet71,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CA10" s="15">
-        <f>COUNTIF(angemeldet72,"X")</f>
+        <f>COUNTIFS(angemeldet72,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CB10" s="15">
-        <f>COUNTIF(angemeldet73,"X")</f>
+        <f>COUNTIFS(angemeldet73,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CC10" s="15">
-        <f>COUNTIF(angemeldet74,"X")</f>
+        <f>COUNTIFS(angemeldet74,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CD10" s="15">
-        <f>COUNTIF(angemeldet75,"X")</f>
+        <f>COUNTIFS(angemeldet75,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CE10" s="15">
-        <f>COUNTIF(angemeldet76,"X")</f>
+        <f>COUNTIFS(angemeldet76,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CF10" s="15">
-        <f>COUNTIF(angemeldet77,"X")</f>
+        <f>COUNTIFS(angemeldet77,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CG10" s="15">
-        <f>COUNTIF(angemeldet78,"X")</f>
+        <f>COUNTIFS(angemeldet78,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CH10" s="15">
-        <f>COUNTIF(angemeldet79,"X")</f>
+        <f>COUNTIFS(angemeldet79,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CI10" s="15">
-        <f>COUNTIF(angemeldet80,"X")</f>
+        <f>COUNTIFS(angemeldet80,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CJ10" s="15">
-        <f>COUNTIF(angemeldet81,"X")</f>
+        <f>COUNTIFS(angemeldet81,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CK10" s="15">
-        <f>COUNTIF(angemeldet82,"X")</f>
+        <f>COUNTIFS(angemeldet82,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CL10" s="15">
-        <f>COUNTIF(angemeldet83,"X")</f>
+        <f>COUNTIFS(angemeldet83,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CM10" s="15">
-        <f>COUNTIF(angemeldet84,"X")</f>
+        <f>COUNTIFS(angemeldet84,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CN10" s="15">
-        <f>COUNTIF(angemeldet85,"X")</f>
+        <f>COUNTIFS(angemeldet85,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CO10" s="15">
-        <f>COUNTIF(angemeldet86,"X")</f>
+        <f>COUNTIFS(angemeldet86,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CP10" s="15">
-        <f>COUNTIF(angemeldet87,"X")</f>
+        <f>COUNTIFS(angemeldet87,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CQ10" s="15">
-        <f>COUNTIF(angemeldet88,"X")</f>
+        <f>COUNTIFS(angemeldet88,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CR10" s="15">
-        <f>COUNTIF(angemeldet89,"X")</f>
+        <f>COUNTIFS(angemeldet89,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CS10" s="15">
-        <f>COUNTIF(angemeldet90,"X")</f>
+        <f>COUNTIFS(angemeldet90,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CT10" s="15">
-        <f>COUNTIF(angemeldet91,"X")</f>
+        <f>COUNTIFS(angemeldet91,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CU10" s="15">
-        <f>COUNTIF(angemeldet92,"X")</f>
+        <f>COUNTIFS(angemeldet92,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CV10" s="15">
-        <f>COUNTIF(angemeldet93,"X")</f>
+        <f>COUNTIFS(angemeldet93,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CW10" s="15">
-        <f>COUNTIF(angemeldet94,"X")</f>
+        <f>COUNTIFS(angemeldet94,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CX10" s="15">
-        <f>COUNTIF(angemeldet95,"X")</f>
+        <f>COUNTIFS(angemeldet95,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CY10" s="15">
-        <f>COUNTIF(angemeldet96,"X")</f>
+        <f>COUNTIFS(angemeldet96,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="CZ10" s="15">
-        <f>COUNTIF(angemeldet97,"X")</f>
+        <f>COUNTIFS(angemeldet97,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="DA10" s="15">
-        <f>COUNTIF(angemeldet98,"X")</f>
+        <f>COUNTIFS(angemeldet98,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="DB10" s="15">
-        <f>COUNTIF(angemeldet99,"X")</f>
+        <f>COUNTIFS(angemeldet99,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
       <c r="DC10" s="15">
-        <f>COUNTIF(angemeldet100,"X")</f>
+        <f>COUNTIFS(angemeldet100,"X",statusKategorie,$B$27)</f>
         <v>0</v>
       </c>
     </row>
@@ -3821,15 +3822,15 @@
       </c>
     </row>
     <row r="12" spans="1:108" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="27">
-        <f>COUNTIF(statusKategorie,$B$30)</f>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="18">
+        <f>COUNTIF(freigegebenKategorie,$B$30)</f>
         <v>0</v>
       </c>
       <c r="G12" s="15"/>

</xml_diff>